<commit_message>
modified karthik's output file
</commit_message>
<xml_diff>
--- a/Karthik'sOutput.xlsx
+++ b/Karthik'sOutput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="113_{2208DE3C-751A-4C9F-8DFA-5DEED3024332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{12AA7BBE-3A56-4690-B430-1A809C489C70}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{DB6E3473-17C4-4963-BBAF-F9CF585A80BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F1ADD60-41D9-4AAD-9ED7-29B9E44F38B9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3A28934A-972A-4B86-9E4B-9B9EF184AD0A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0DADBE3E-F64E-41F2-A8FF-CEFADDBA6D98}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>"3. For the days selected in step two, identify all emails which denote a change detected. Open each email and ensure the details within (e.g. each change is captured within the monthly tracker (findings tab)."</t>
   </si>
@@ -63,6 +63,12 @@
     <t>Selection 2 (Date)</t>
   </si>
   <si>
+    <t>magic_kq_023</t>
+  </si>
+  <si>
+    <t>magic_kl02</t>
+  </si>
+  <si>
     <t>Selection 3 (Date)</t>
   </si>
   <si>
@@ -97,12 +103,6 @@
   </si>
   <si>
     <t>oiuer3298</t>
-  </si>
-  <si>
-    <t>magic_kq_023</t>
-  </si>
-  <si>
-    <t>magic_kl02</t>
   </si>
 </sst>
 </file>
@@ -454,16 +454,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4602C9DE-E17E-477F-82EF-344C56581430}">
-  <dimension ref="A26:H94"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0A8D42-1879-4AEB-A0E7-553672732688}">
+  <dimension ref="A26:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -492,7 +490,6 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D29" s="1"/>
       <c r="H29" t="s">
         <v>5</v>
       </c>
@@ -524,7 +521,7 @@
         <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
@@ -534,12 +531,12 @@
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H34" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -554,17 +551,17 @@
         <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H36" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
@@ -579,42 +576,27 @@
         <v>4</v>
       </c>
       <c r="H37" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H38" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="1">
-        <v>43844</v>
-      </c>
-      <c r="E39" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39">
-        <v>9</v>
-      </c>
       <c r="H39" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H40" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -629,197 +611,17 @@
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H42" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H43" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="1">
-        <v>43854</v>
-      </c>
-      <c r="E44" t="s">
-        <v>3</v>
-      </c>
-      <c r="G44">
-        <v>16</v>
-      </c>
-      <c r="H44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H45" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" t="s">
-        <v>2</v>
-      </c>
-      <c r="D46" s="1">
-        <v>43844</v>
-      </c>
-      <c r="E46" t="s">
-        <v>3</v>
-      </c>
-      <c r="G46">
-        <v>9</v>
-      </c>
-      <c r="H46" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H47" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D48" s="1">
-        <v>43852</v>
-      </c>
-      <c r="E48" t="s">
-        <v>3</v>
-      </c>
-      <c r="G48">
-        <v>13</v>
-      </c>
-      <c r="H48" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H49" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H50" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H51" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B61" t="s">
-        <v>17</v>
-      </c>
-      <c r="C61" t="s">
-        <v>2</v>
-      </c>
-      <c r="D61" s="1">
-        <v>43854</v>
-      </c>
-      <c r="E61" t="s">
-        <v>3</v>
-      </c>
-      <c r="G61">
-        <v>16</v>
-      </c>
-      <c r="H61" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H62" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H63" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" t="s">
-        <v>2</v>
-      </c>
-      <c r="D67" s="1">
-        <v>43852</v>
-      </c>
-      <c r="E67" t="s">
-        <v>3</v>
-      </c>
-      <c r="G67">
-        <v>13</v>
-      </c>
-      <c r="H67" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H68" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H69" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H70" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B92" t="s">
-        <v>17</v>
-      </c>
-      <c r="C92" t="s">
-        <v>2</v>
-      </c>
-      <c r="D92" s="1">
-        <v>43854</v>
-      </c>
-      <c r="E92" t="s">
-        <v>3</v>
-      </c>
-      <c r="G92">
-        <v>16</v>
-      </c>
-      <c r="H92" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H93" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H94" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -828,7 +630,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2576A46B-7317-4470-BDEF-7D6807DB2678}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB1240E-58D9-45D8-A587-A9DDFF24EFD9}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>